<commit_message>
Copy Files From Source Repo (2025-01-24 17:04)
</commit_message>
<xml_diff>
--- a/ResourceFiles/Charger_sales_report_2022-2024.xlsx
+++ b/ResourceFiles/Charger_sales_report_2022-2024.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/maquinl_microsoft_com/Documents/Desktop/Jan Updates/MS-4012/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C194DB79-7777-4DC8-80FD-E37B2865CB3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2725CB42-44FD-4FA0-90C7-155855583B25}"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="1380" windowWidth="31380" windowHeight="16605" activeTab="0"/>
+    <workbookView xWindow="10860" yWindow="1380" windowWidth="31380" windowHeight="16605" xr2:uid="{01136639-D56C-4CEF-AF0E-AA7A37846DA8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Report delle vendite" sheetId="1" r:id="rId3"/>
+    <sheet name="Sales report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,194 +38,62 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Anno-Trimestre</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Midwest</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Mountain</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Northeast</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>South</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>sud-orientale</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>West</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2022-T1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2022-T2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2022-T3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2022-T4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2023-T1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2023-T2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2023-T3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2023-T4</t>
-    </r>
+    <t>Year-Quarter</t>
+  </si>
+  <si>
+    <t>Midwest</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>Northeast</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>Southeast</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>2022-Q1</t>
+  </si>
+  <si>
+    <t>2022-Q2</t>
+  </si>
+  <si>
+    <t>2022-Q3</t>
+  </si>
+  <si>
+    <t>2022-Q4</t>
+  </si>
+  <si>
+    <t>2023-Q1</t>
+  </si>
+  <si>
+    <t>2023-Q2</t>
+  </si>
+  <si>
+    <t>2023-Q3</t>
+  </si>
+  <si>
+    <t>2023-Q4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -245,111 +113,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -677,16 +451,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A438346-8F95-46E3-9ED8-B0FC129AAD99}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A438346-8F95-46E3-9ED8-B0FC129AAD99}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="B2" sqref="B2:G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -709,7 +483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -732,7 +506,7 @@
         <v>392986</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -755,7 +529,7 @@
         <v>389381</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -778,7 +552,7 @@
         <v>407447</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -801,7 +575,7 @@
         <v>414736</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -824,7 +598,7 @@
         <v>385445</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -847,7 +621,7 @@
         <v>392426</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -870,7 +644,7 @@
         <v>411466</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -896,4 +670,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{87ba5c36-b7cf-4793-bbc2-bd5b3a9f95ca}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Copy Files From Source Repo (2025-02-05 17:04)
</commit_message>
<xml_diff>
--- a/ResourceFiles/Charger_sales_report_2022-2024.xlsx
+++ b/ResourceFiles/Charger_sales_report_2022-2024.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/maquinl_microsoft_com/Documents/Desktop/Jan Updates/MS-4012/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C194DB79-7777-4DC8-80FD-E37B2865CB3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2725CB42-44FD-4FA0-90C7-155855583B25}"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="1380" windowWidth="31380" windowHeight="16605" activeTab="0"/>
+    <workbookView xWindow="10860" yWindow="1380" windowWidth="31380" windowHeight="16605" xr2:uid="{01136639-D56C-4CEF-AF0E-AA7A37846DA8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Report delle vendite" sheetId="1" r:id="rId3"/>
+    <sheet name="Sales report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,194 +38,62 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Anno-Trimestre</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Midwest</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Mountain</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Northeast</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>South</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>sud-orientale</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>West</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2022-T1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2022-T2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2022-T3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2022-T4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2023-T1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2023-T2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2023-T3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>2023-T4</t>
-    </r>
+    <t>Year-Quarter</t>
+  </si>
+  <si>
+    <t>Midwest</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>Northeast</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>Southeast</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>2022-Q1</t>
+  </si>
+  <si>
+    <t>2022-Q2</t>
+  </si>
+  <si>
+    <t>2022-Q3</t>
+  </si>
+  <si>
+    <t>2022-Q4</t>
+  </si>
+  <si>
+    <t>2023-Q1</t>
+  </si>
+  <si>
+    <t>2023-Q2</t>
+  </si>
+  <si>
+    <t>2023-Q3</t>
+  </si>
+  <si>
+    <t>2023-Q4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -245,111 +113,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -677,16 +451,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A438346-8F95-46E3-9ED8-B0FC129AAD99}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A438346-8F95-46E3-9ED8-B0FC129AAD99}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="B2" sqref="B2:G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -709,7 +483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -732,7 +506,7 @@
         <v>392986</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -755,7 +529,7 @@
         <v>389381</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -778,7 +552,7 @@
         <v>407447</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -801,7 +575,7 @@
         <v>414736</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -824,7 +598,7 @@
         <v>385445</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -847,7 +621,7 @@
         <v>392426</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -870,7 +644,7 @@
         <v>411466</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -896,4 +670,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{87ba5c36-b7cf-4793-bbc2-bd5b3a9f95ca}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>